<commit_message>
Change in 2022/8/14(FolderName change:sapu -> supu)
</commit_message>
<xml_diff>
--- a/supu/Excel_Concerned/output.xlsx
+++ b/supu/Excel_Concerned/output.xlsx
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>35058</v>
+        <v>94547</v>
       </c>
     </row>
     <row r="3">
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>40995</v>
+        <v>59346</v>
       </c>
     </row>
     <row r="4">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>70372</v>
+        <v>83076</v>
       </c>
     </row>
     <row r="5">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>54606</v>
+        <v>26068</v>
       </c>
     </row>
     <row r="6">
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>58212</v>
+        <v>55861</v>
       </c>
     </row>
     <row r="7">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>49237</v>
+        <v>28547</v>
       </c>
     </row>
     <row r="8">
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>27207</v>
+        <v>11840</v>
       </c>
     </row>
     <row r="9">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>12480</v>
+        <v>41102</v>
       </c>
     </row>
     <row r="10">
@@ -836,7 +836,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>65283</v>
+        <v>87681</v>
       </c>
     </row>
     <row r="11">
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>91432</v>
+        <v>15646</v>
       </c>
     </row>
     <row r="12">
@@ -856,7 +856,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>84251</v>
+        <v>35703</v>
       </c>
     </row>
     <row r="13">
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>20848</v>
+        <v>87336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>